<commit_message>
hai ca se poate
</commit_message>
<xml_diff>
--- a/Cerinte Proiect 2 .xlsx
+++ b/Cerinte Proiect 2 .xlsx
@@ -630,8 +630,8 @@
   </sheetPr>
   <dimension ref="A1:F1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>